<commit_message>
add try/catch for cathing error in the error message will not apear
</commit_message>
<xml_diff>
--- a/src/main/resources/emails.xlsx
+++ b/src/main/resources/emails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciejwachowski/Desktop/repo_priv/Esky_selenium_java/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B183A7B1-0B73-B54E-8399-065210501747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D619A-22E4-564D-A338-D18536B7B58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="58120" yWindow="3340" windowWidth="28040" windowHeight="17440" xr2:uid="{00E69155-4AA3-1041-BB4D-EE28248921A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>maciek@</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>IncorrectEmails</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>maciek@example.com</t>
   </si>
 </sst>
 </file>
@@ -101,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37998BE-2694-F64F-9303-38012694539A}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,7 +439,7 @@
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -448,8 +455,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -464,6 +474,9 @@
       </c>
       <c r="E2" t="s">
         <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>